<commit_message>
Add Julia set timings
</commit_message>
<xml_diff>
--- a/CPlusPlus/Tbb/timings.xlsx
+++ b/CPlusPlus/Tbb/timings.xlsx
@@ -9,15 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="0" windowWidth="27615" windowHeight="12885" activeTab="1"/>
+    <workbookView xWindow="2370" yWindow="0" windowWidth="27615" windowHeight="12885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fibonacci" sheetId="1" r:id="rId1"/>
-    <sheet name="trees" sheetId="2" r:id="rId2"/>
+    <sheet name="julia_set" sheetId="3" r:id="rId2"/>
+    <sheet name="trees" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="fibonacci_tasks" localSheetId="0">fibonacci!$A$1:$B$13</definedName>
-    <definedName name="tree_sum" localSheetId="1">trees!$A$1:$B$13</definedName>
+    <definedName name="timings_1" localSheetId="1">julia_set!$A$1:$E$13</definedName>
+    <definedName name="tree_sum" localSheetId="2">trees!$A$1:$B$13</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +40,16 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="tree_sum" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" name="timings" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\geert\Downloads\timings.txt" space="1" consecutive="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="tree_sum" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\geert\Documents\Data\GitHub\training-material\CPlusPlus\Tbb\Tree\tree_sum.txt" space="1" consecutive="1">
       <textFields count="2">
         <textField/>
@@ -50,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>cores</t>
   </si>
@@ -62,6 +73,24 @@
   </si>
   <si>
     <t>speedup</t>
+  </si>
+  <si>
+    <t>omp speedup</t>
+  </si>
+  <si>
+    <t>omp walltime</t>
+  </si>
+  <si>
+    <t>omp efficiency</t>
+  </si>
+  <si>
+    <t>tbb walltime</t>
+  </si>
+  <si>
+    <t>tbb speedup</t>
+  </si>
+  <si>
+    <t>tbb efficiency</t>
   </si>
 </sst>
 </file>
@@ -1275,6 +1304,1123 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>speedup</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>julia_set!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omp speedup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>julia_set!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>julia_set!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>8.3984771573604071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7676056338028179</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.320796460176993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.9729241877256323</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5204918032786887</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0902348578491967</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1335227272727275</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3926247288503255</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0824417872876024</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9138230190861774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.900631820792648</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6AFC-426A-B724-2B858A10344F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>julia_set!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tbb speedup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>julia_set!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>julia_set!$F$2:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>23.805755395683459</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.060000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.348387096774196</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.234375000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.236000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.076642335766424</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.7899408284023686</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0254777070063703</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.3370967741935491</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6362637362637367</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8897772701313535</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6AFC-426A-B724-2B858A10344F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="531705672"/>
+        <c:axId val="531698784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="531705672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="531698784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="531698784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="531705672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>efficiency</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>julia_set!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omp efficiency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>julia_set!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>julia_set!$D$2:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.23329103214890021</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24273767605633806</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24402654867256643</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24887184115523467</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25113843351548271</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25563967861557479</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26112689393939398</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29907809110629069</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.34707363121460039</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.47845575477154434</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95031591039632402</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1144-4203-B6AF-CB7F30B3021C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>julia_set!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tbb efficiency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>julia_set!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>julia_set!$G$2:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.66127098321342936</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68937500000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7116129032258065</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.71809895833333348</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73533333333333339</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75479014598540151</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.81582840236686405</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.87818471337579629</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.88951612903225818</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.90906593406593417</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.94488863506567677</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1144-4203-B6AF-CB7F30B3021C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="535746576"/>
+        <c:axId val="535743624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="535746576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="535743624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="535743624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="535746576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>walltime</a:t>
             </a:r>
           </a:p>
@@ -1631,7 +2777,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1997,7 +3143,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2603,6 +3749,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5184,6 +6410,1038 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5798,6 +8056,71 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>347662</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>252412</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>147637</xdr:colOff>
       <xdr:row>4</xdr:row>
@@ -5894,7 +8217,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tree_sum" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="timings_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tree_sum" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6387,9 +8714,382 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" activeCellId="2" sqref="A1:A1048576 D1:D1048576 G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>3.94</v>
+      </c>
+      <c r="C2">
+        <f>B$13/B2</f>
+        <v>8.3984771573604071</v>
+      </c>
+      <c r="D2">
+        <f>C2/A2</f>
+        <v>0.23329103214890021</v>
+      </c>
+      <c r="E2">
+        <v>1.39</v>
+      </c>
+      <c r="F2">
+        <f>E$13/E2</f>
+        <v>23.805755395683459</v>
+      </c>
+      <c r="G2">
+        <f>F2/A2</f>
+        <v>0.66127098321342936</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>4.26</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C13" si="0">B$13/B3</f>
+        <v>7.7676056338028179</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D13" si="1">C3/A3</f>
+        <v>0.24273767605633806</v>
+      </c>
+      <c r="E3">
+        <v>1.5</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F13" si="2">E$13/E3</f>
+        <v>22.060000000000002</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G12" si="3">F3/A3</f>
+        <v>0.68937500000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>7.320796460176993</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>0.24402654867256643</v>
+      </c>
+      <c r="E4">
+        <v>1.55</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>21.348387096774196</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="3"/>
+        <v>0.7116129032258065</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>5.54</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>5.9729241877256323</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>0.24887184115523467</v>
+      </c>
+      <c r="E5">
+        <v>1.92</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>17.234375000000004</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>0.71809895833333348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>7.32</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>4.5204918032786887</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>0.25113843351548271</v>
+      </c>
+      <c r="E6">
+        <v>2.5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>13.236000000000001</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>0.73533333333333339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>8.09</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>4.0902348578491967</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>0.25563967861557479</v>
+      </c>
+      <c r="E7">
+        <v>2.74</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>12.076642335766424</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>0.75479014598540151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>10.56</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>3.1335227272727275</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0.26112689393939398</v>
+      </c>
+      <c r="E8">
+        <v>3.38</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>9.7899408284023686</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>0.81582840236686405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>13.83</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2.3926247288503255</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0.29907809110629069</v>
+      </c>
+      <c r="E9">
+        <v>4.71</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>7.0254777070063703</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>0.87818471337579629</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>15.89</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2.0824417872876024</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>0.34707363121460039</v>
+      </c>
+      <c r="E10">
+        <v>6.2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>5.3370967741935491</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>0.88951612903225818</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>17.29</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>1.9138230190861774</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>0.47845575477154434</v>
+      </c>
+      <c r="E11">
+        <v>9.1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>3.6362637362637367</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>0.90906593406593417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>17.41</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>1.900631820792648</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>0.95031591039632402</v>
+      </c>
+      <c r="E12">
+        <v>17.510000000000002</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>1.8897772701313535</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>0.94488863506567677</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>33.090000000000003</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>33.090000000000003</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G3:G13" si="4">F13/D13</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" activeCellId="1" sqref="A1:A1048576 D1:D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>